<commit_message>
Updating midterm exam and data
</commit_message>
<xml_diff>
--- a/Assignments/Midterm-Exam/Nursing VR Study.xlsx
+++ b/Assignments/Midterm-Exam/Nursing VR Study.xlsx
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="C16">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="C18">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19">
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="C20">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="C22">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="C23">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24">
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="C24">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="C26">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="C27">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="C28">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="C29">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C30">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="C31">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
@@ -836,7 +836,7 @@
         </is>
       </c>
       <c r="C32">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34">
@@ -881,7 +881,7 @@
         </is>
       </c>
       <c r="C35">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36">
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="C36">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37">
@@ -911,7 +911,7 @@
         </is>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="C39">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40">
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="C40">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41">
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="C41">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>